<commit_message>
Update base volunteer sheet
</commit_message>
<xml_diff>
--- a/swing_devils.xlsx
+++ b/swing_devils.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kedot\Documents\Python Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kedot\Documents\Python Scripts\Swing-Devils-Volunteer-Randomizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C0C49B3-2B50-45B4-BAEE-B250F89FE25E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA7D603-236C-479F-B160-BD0681C9A066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{F5DEDD0F-8B25-4966-8B90-FA52C43EABE8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
   <si>
     <t>DATE:</t>
   </si>
@@ -45,33 +45,15 @@
     <t>Setup/open</t>
   </si>
   <si>
-    <t>Taylor</t>
-  </si>
-  <si>
-    <t>Jessica</t>
-  </si>
-  <si>
     <t>Teaching Lesson</t>
   </si>
   <si>
     <t>Begin</t>
   </si>
   <si>
-    <t>Geoff and Katrina</t>
-  </si>
-  <si>
-    <t>Madeline and Mariah</t>
-  </si>
-  <si>
     <t>Series</t>
   </si>
   <si>
-    <t>Geoff</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
     <t>Teaching lesson</t>
   </si>
   <si>
@@ -81,39 +63,21 @@
     <t>DJ</t>
   </si>
   <si>
-    <t>Mariah</t>
-  </si>
-  <si>
     <t>First door shift 6:45</t>
   </si>
   <si>
     <t>Closing</t>
   </si>
   <si>
-    <t>Courtney</t>
-  </si>
-  <si>
-    <t>Michael</t>
-  </si>
-  <si>
-    <t>Close at 9:30 PM</t>
-  </si>
-  <si>
     <t>Tear Down</t>
   </si>
   <si>
     <t>Till Count</t>
   </si>
   <si>
-    <t>Doty</t>
-  </si>
-  <si>
     <t>Notes:</t>
   </si>
   <si>
-    <t>School Spirit Dance</t>
-  </si>
-  <si>
     <t>Board Meeting 6pm</t>
   </si>
   <si>
@@ -126,19 +90,13 @@
     <t>Facebook</t>
   </si>
   <si>
-    <t>Mariah and Courtney</t>
-  </si>
-  <si>
-    <t>Courtney and Madeline</t>
-  </si>
-  <si>
-    <t>Madeline</t>
-  </si>
-  <si>
-    <t>Eric</t>
-  </si>
-  <si>
-    <t>Halloween Night!</t>
+    <t>Close at 9:00 PM</t>
+  </si>
+  <si>
+    <t>Masquerade Dance</t>
+  </si>
+  <si>
+    <t>Live Band</t>
   </si>
 </sst>
 </file>
@@ -185,7 +143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,73 +164,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF1C232"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF00A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF683A79"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6D9EEB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF008B84"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE10000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7EE012"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE69138"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF38761D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA64D79"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -324,58 +216,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -691,33 +544,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C603D7FA-415A-49BD-8162-4B277692B605}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21660B6F-AA22-48AC-A7CB-1CD749E94B77}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="10.46484375" customWidth="1"/>
-    <col min="3" max="3" width="8.19921875" customWidth="1"/>
-    <col min="4" max="4" width="12.46484375" customWidth="1"/>
-    <col min="6" max="6" width="8.06640625" customWidth="1"/>
-    <col min="7" max="7" width="6.53125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="19.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:9" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4">
-        <v>43713</v>
+        <v>43741</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="4">
-        <v>43720</v>
+        <v>43748</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="5"/>
@@ -725,7 +573,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="3">
-        <v>43721</v>
+        <v>43749</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
@@ -747,17 +595,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="7"/>
-      <c r="B3" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="B3" s="7"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="H3" s="14">
+      <c r="H3" s="12">
         <v>0.77083333333333337</v>
       </c>
       <c r="I3" s="5"/>
@@ -776,55 +620,47 @@
     <row r="5" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="B5" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>8</v>
-      </c>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>9</v>
-      </c>
+      <c r="D6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>11</v>
-      </c>
+      <c r="A7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>12</v>
-      </c>
+      <c r="D7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="7"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I7" s="5"/>
     </row>
@@ -837,19 +673,19 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
       <c r="B9" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -858,18 +694,14 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="5"/>
-      <c r="B10" s="18" t="s">
-        <v>11</v>
-      </c>
+      <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I10" s="5"/>
     </row>
@@ -887,30 +719,26 @@
     <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="5"/>
       <c r="B12" s="9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="5"/>
-      <c r="B13" s="22" t="s">
-        <v>19</v>
-      </c>
+      <c r="B13" s="7"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="23" t="s">
-        <v>20</v>
-      </c>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -925,19 +753,19 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="5"/>
       <c r="B15" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -945,72 +773,64 @@
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="A16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>11</v>
-      </c>
+      <c r="D16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>24</v>
-      </c>
+      <c r="A17" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>24</v>
-      </c>
+      <c r="D17" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" ht="43.15" x14ac:dyDescent="0.5">
-      <c r="A18" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>26</v>
+      <c r="A18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="15" t="s">
-        <v>25</v>
+      <c r="D18" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+      <c r="B19" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="25" t="s">
-        <v>29</v>
-      </c>
+      <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -1018,32 +838,32 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+      <c r="B20" s="16" t="s">
+        <v>17</v>
+      </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I20" s="21" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="4">
-        <v>43727</v>
+        <v>43755</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E21" s="4">
-        <v>43734</v>
+        <v>43762</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="5"/>
@@ -1067,14 +887,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="5"/>
-      <c r="B23" s="18" t="s">
-        <v>11</v>
-      </c>
+      <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="23" t="s">
-        <v>20</v>
-      </c>
+      <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -1094,51 +910,43 @@
     <row r="25" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="5"/>
       <c r="B25" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A26" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>31</v>
-      </c>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A26" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>32</v>
-      </c>
+      <c r="D26" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A27" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>12</v>
-      </c>
+      <c r="A27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="5"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>12</v>
-      </c>
+      <c r="D27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
@@ -1158,12 +966,12 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="5"/>
       <c r="B29" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -1172,14 +980,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="5"/>
-      <c r="B30" s="26" t="s">
-        <v>33</v>
-      </c>
+      <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
@@ -1199,12 +1003,12 @@
     <row r="32" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32" s="5"/>
       <c r="B32" s="9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -1213,14 +1017,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="5"/>
-      <c r="B33" s="23" t="s">
-        <v>20</v>
-      </c>
+      <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
@@ -1240,12 +1040,12 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="5"/>
       <c r="B35" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -1253,51 +1053,43 @@
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="23" t="s">
-        <v>20</v>
-      </c>
+      <c r="A36" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="5"/>
       <c r="C36" s="5"/>
-      <c r="D36" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" s="27" t="s">
-        <v>34</v>
-      </c>
+      <c r="D36" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A37" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="24" t="s">
-        <v>24</v>
-      </c>
+      <c r="A37" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="5"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="24" t="s">
-        <v>24</v>
-      </c>
+      <c r="D37" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A38" s="15" t="s">
-        <v>25</v>
+      <c r="A38" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="28" t="s">
-        <v>25</v>
+      <c r="D38" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -1331,7 +1123,7 @@
       <c r="A41" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="1"/>
+      <c r="B41" s="4"/>
       <c r="C41" s="1"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -1378,7 +1170,7 @@
     <row r="45" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A45" s="5"/>
       <c r="B45" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -1389,8 +1181,8 @@
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A46" s="15" t="s">
-        <v>7</v>
+      <c r="A46" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="5"/>
@@ -1402,12 +1194,10 @@
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A47" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>12</v>
-      </c>
+      <c r="A47" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
@@ -1430,7 +1220,7 @@
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="5"/>
       <c r="B49" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -1465,7 +1255,7 @@
     <row r="52" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A52" s="5"/>
       <c r="B52" s="9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -1500,7 +1290,7 @@
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="5"/>
       <c r="B55" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -1511,8 +1301,8 @@
       <c r="I55" s="5"/>
     </row>
     <row r="56" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A56" s="15" t="s">
-        <v>22</v>
+      <c r="A56" s="13" t="s">
+        <v>12</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -1524,8 +1314,8 @@
       <c r="I56" s="5"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A57" s="15" t="s">
-        <v>23</v>
+      <c r="A57" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="B57" s="7"/>
       <c r="C57" s="5"/>
@@ -1536,13 +1326,11 @@
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
     </row>
-    <row r="58" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A58" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B58" s="29" t="s">
-        <v>35</v>
-      </c>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A58" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
@@ -1575,6 +1363,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New sheet made for December
</commit_message>
<xml_diff>
--- a/swing_devils.xlsx
+++ b/swing_devils.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kedot\Documents\Python Scripts\Swing-Devils-Volunteer-Randomizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA7D603-236C-479F-B160-BD0681C9A066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C95AB63-6624-4F2F-B4AD-E026D60A37DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{F5DEDD0F-8B25-4966-8B90-FA52C43EABE8}"/>
   </bookViews>
@@ -93,10 +93,10 @@
     <t>Close at 9:00 PM</t>
   </si>
   <si>
-    <t>Masquerade Dance</t>
-  </si>
-  <si>
     <t>Live Band</t>
+  </si>
+  <si>
+    <t>Holiday Ugly Sweater Dance</t>
   </si>
 </sst>
 </file>
@@ -181,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -229,6 +229,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -547,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21660B6F-AA22-48AC-A7CB-1CD749E94B77}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -802,18 +805,18 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="43.15" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" ht="28.9" x14ac:dyDescent="0.5">
       <c r="A18" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="14" t="s">
         <v>15</v>
       </c>
       <c r="F18" s="5"/>
@@ -826,11 +829,13 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="5"/>
       <c r="B19" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="E19" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -838,9 +843,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="5"/>
-      <c r="B20" s="16" t="s">
-        <v>17</v>
-      </c>
+      <c r="B20" s="17"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1252,7 +1255,7 @@
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
     </row>
-    <row r="52" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="5"/>
       <c r="B52" s="9" t="s">
         <v>10</v>
@@ -1300,7 +1303,7 @@
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
     </row>
-    <row r="56" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="13" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Update January volunteer sheet
</commit_message>
<xml_diff>
--- a/swing_devils.xlsx
+++ b/swing_devils.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kedot\Documents\Python Scripts\Swing-Devils-Volunteer-Randomizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C95AB63-6624-4F2F-B4AD-E026D60A37DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14BCC2D-63D8-4D53-8842-0DAEA0B3C490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{F5DEDD0F-8B25-4966-8B90-FA52C43EABE8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="22">
   <si>
     <t>DATE:</t>
   </si>
@@ -78,25 +78,25 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>Board Meeting 6pm</t>
-  </si>
-  <si>
     <t>Monthly Duties</t>
   </si>
   <si>
-    <t>Tables</t>
-  </si>
-  <si>
     <t>Facebook</t>
   </si>
   <si>
     <t>Close at 9:00 PM</t>
   </si>
   <si>
-    <t>Live Band</t>
-  </si>
-  <si>
-    <t>Holiday Ugly Sweater Dance</t>
+    <t>Geoff</t>
+  </si>
+  <si>
+    <t>Colby</t>
+  </si>
+  <si>
+    <t>Jedediah</t>
+  </si>
+  <si>
+    <t>Board Meeting 7pm at Karma</t>
   </si>
 </sst>
 </file>
@@ -143,7 +143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +168,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008B84"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF93C47D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD5A6BD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -181,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -222,16 +240,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -547,28 +571,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21660B6F-AA22-48AC-A7CB-1CD749E94B77}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC3CFF3E-4AB1-43ED-9F39-C30B29A60526}">
   <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="26.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.59765625" customWidth="1"/>
+    <col min="3" max="3" width="5.86328125" customWidth="1"/>
+    <col min="4" max="4" width="13.86328125" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" customWidth="1"/>
+    <col min="7" max="7" width="8.06640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4">
-        <v>43741</v>
+        <v>43804</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="4">
-        <v>43748</v>
+        <v>43811</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="5"/>
@@ -576,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="3">
-        <v>43749</v>
+        <v>43812</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
@@ -607,7 +638,9 @@
       <c r="H3" s="12">
         <v>0.77083333333333337</v>
       </c>
-      <c r="I3" s="5"/>
+      <c r="I3" s="16" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
@@ -618,7 +651,9 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="I4" s="17" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
@@ -678,7 +713,9 @@
       <c r="H8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="5"/>
+      <c r="I8" s="18" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
@@ -734,9 +771,11 @@
       <c r="H12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I12" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="5"/>
       <c r="B13" s="7"/>
       <c r="C13" s="5"/>
@@ -744,10 +783,14 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="H13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -755,9 +798,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
@@ -805,53 +846,47 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="28.9" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" ht="57.4" x14ac:dyDescent="0.5">
       <c r="A18" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>15</v>
-      </c>
+      <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="5"/>
-      <c r="B19" s="16" t="s">
-        <v>20</v>
-      </c>
+      <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="14" t="s">
-        <v>17</v>
-      </c>
+      <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="11"/>
+      <c r="H19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="5"/>
-      <c r="B20" s="17"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
@@ -859,14 +894,14 @@
         <v>0</v>
       </c>
       <c r="B21" s="4">
-        <v>43755</v>
+        <v>43818</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E21" s="4">
-        <v>43762</v>
+        <v>43825</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="5"/>
@@ -1091,10 +1126,10 @@
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E38" s="5"/>
+      <c r="E38" s="13"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
@@ -1126,7 +1161,7 @@
       <c r="A41" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="4"/>
+      <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -1255,7 +1290,7 @@
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A52" s="5"/>
       <c r="B52" s="9" t="s">
         <v>10</v>
@@ -1303,7 +1338,7 @@
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A56" s="13" t="s">
         <v>12</v>
       </c>

</xml_diff>